<commit_message>
updating files and folders
</commit_message>
<xml_diff>
--- a/data-raw/table_affix_nondet.xlsx
+++ b/data-raw/table_affix_nondet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\skripsi2\kStemInd\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rumah\skripsilah-sebelum-diskripsikan\_algoritma\kStemInd\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="5250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="5250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="suffixes" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,11 +886,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -898,7 +898,7 @@
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -916,7 +916,7 @@
       </c>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>162</v>
       </c>
@@ -934,7 +934,7 @@
       </c>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>162</v>
       </c>
@@ -952,7 +952,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>162</v>
       </c>
@@ -970,7 +970,7 @@
       </c>
       <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>123</v>
       </c>
@@ -988,7 +988,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>123</v>
       </c>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>123</v>
       </c>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>127</v>
       </c>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>127</v>
       </c>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>127</v>
       </c>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="8"/>
       <c r="C11" s="2"/>
@@ -1086,7 +1086,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="8"/>
       <c r="C12" s="2"/>
@@ -1094,7 +1094,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="8"/>
       <c r="C13" s="2"/>
@@ -1102,7 +1102,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="8"/>
       <c r="C14" s="2"/>
@@ -1110,7 +1110,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="8"/>
       <c r="C15" s="2"/>
@@ -1118,7 +1118,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="8"/>
       <c r="C16" s="2"/>
@@ -1126,7 +1126,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="8"/>
       <c r="C17" s="2"/>
@@ -1134,7 +1134,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="8"/>
       <c r="C18" s="2"/>
@@ -1142,7 +1142,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="8"/>
       <c r="C19" s="2"/>
@@ -1150,7 +1150,7 @@
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="8"/>
       <c r="C20" s="2"/>
@@ -1168,11 +1168,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
@@ -1182,7 +1182,7 @@
     <col min="6" max="6" width="11" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>131</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>131</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>132</v>
       </c>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>132</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>132</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>132</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>133</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>133</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>133</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>133</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>134</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>134</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>134</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>135</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>135</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>135</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>135</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>135</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>136</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>136</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>137</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>137</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>137</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>137</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>138</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>138</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>138</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>139</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>139</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>139</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>21</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>21</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>21</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>21</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>140</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>140</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>140</v>
       </c>
@@ -2005,7 +2005,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>22</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>141</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>141</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>141</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>141</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -2119,7 +2119,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -2136,48 +2136,48 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C62" s="2"/>
     </row>
   </sheetData>
@@ -2194,14 +2194,14 @@
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>142</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>143</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>143</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>143</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>143</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>143</v>
       </c>
@@ -2299,7 +2299,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>143</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>143</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>143</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>143</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>143</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>144</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>144</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>144</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>144</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>144</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>144</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>144</v>
       </c>

</xml_diff>